<commit_message>
Updated for latest meeting
</commit_message>
<xml_diff>
--- a/Attendance.xlsx
+++ b/Attendance.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17766"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Jakub</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>01-mars</t>
+  </si>
+  <si>
+    <t>15-mars</t>
   </si>
 </sst>
 </file>
@@ -65,7 +68,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-40C]d\-mmm;@"/>
+    <numFmt numFmtId="164" formatCode="[$-40C]d\-mmm;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -99,7 +102,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -118,16 +121,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="B3:D14" totalsRowShown="0">
-  <autoFilter ref="B3:D14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="B3:E14" totalsRowShown="0">
+  <autoFilter ref="B3:E14">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
-  <tableColumns count="3">
+  <tableColumns count="4">
     <tableColumn id="1" name="Colonne1"/>
     <tableColumn id="2" name="21-févr."/>
     <tableColumn id="3" name="01-mars"/>
+    <tableColumn id="4" name="15-mars"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -396,10 +401,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:D14"/>
+  <dimension ref="B3:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -409,7 +414,7 @@
     <col min="4" max="4" width="7.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>10</v>
       </c>
@@ -419,8 +424,11 @@
       <c r="D3" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E3" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>8</v>
       </c>
@@ -430,8 +438,11 @@
       <c r="D4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>1</v>
       </c>
@@ -441,8 +452,11 @@
       <c r="D5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>5</v>
       </c>
@@ -452,8 +466,11 @@
       <c r="D6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E6">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>6</v>
       </c>
@@ -463,8 +480,11 @@
       <c r="D7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>7</v>
       </c>
@@ -474,8 +494,11 @@
       <c r="D8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>4</v>
       </c>
@@ -485,8 +508,11 @@
       <c r="D9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>2</v>
       </c>
@@ -496,8 +522,11 @@
       <c r="D10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>0</v>
       </c>
@@ -507,8 +536,11 @@
       <c r="D11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>3</v>
       </c>
@@ -518,8 +550,11 @@
       <c r="D12">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>9</v>
       </c>
@@ -529,9 +564,12 @@
       <c r="D14">
         <v>1</v>
       </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C4:D14">
+  <conditionalFormatting sqref="C4:E14">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>